<commit_message>
Modified README, deleted scrap R file, organised spacer_entry files
</commit_message>
<xml_diff>
--- a/spacers/original_data/spacer_entry_T1.xlsx
+++ b/spacers/original_data/spacer_entry_T1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="820" yWindow="460" windowWidth="11860" windowHeight="18680" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="820" yWindow="460" windowWidth="13180" windowHeight="18680" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1-clone" sheetId="1" r:id="rId1"/>
@@ -572,6 +572,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -581,7 +582,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -932,8 +932,8 @@
   <dimension ref="A1:L86"/>
   <sheetViews>
     <sheetView zoomScale="119" zoomScaleNormal="119" zoomScalePageLayoutView="119" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C87" sqref="C87"/>
+      <pane ySplit="2" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -944,21 +944,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="E1" s="13" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="E1" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -1002,7 +1002,9 @@
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="6">
+        <v>0</v>
+      </c>
       <c r="C3" s="9">
         <v>1</v>
       </c>
@@ -1047,13 +1049,15 @@
       <c r="A4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
       <c r="C4" s="9">
         <v>4</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D14" si="8">SUM(B4:C4)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
@@ -1073,11 +1077,11 @@
       </c>
       <c r="I4">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" s="3">
         <f t="shared" si="6"/>
@@ -1092,7 +1096,9 @@
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
       <c r="C5" s="9">
         <v>5</v>
       </c>
@@ -1137,7 +1143,9 @@
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="10">
+        <v>0</v>
+      </c>
       <c r="C6" s="9">
         <v>1</v>
       </c>
@@ -1182,7 +1190,9 @@
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="10">
+        <v>0</v>
+      </c>
       <c r="C7" s="9">
         <v>1</v>
       </c>
@@ -1227,7 +1237,9 @@
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="10">
+        <v>0</v>
+      </c>
       <c r="C8" s="9">
         <v>1</v>
       </c>
@@ -1272,7 +1284,9 @@
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="6"/>
+      <c r="B9" s="10">
+        <v>0</v>
+      </c>
       <c r="C9" s="9">
         <v>2</v>
       </c>
@@ -1317,7 +1331,9 @@
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="10">
+        <v>0</v>
+      </c>
       <c r="C10" s="9">
         <v>2</v>
       </c>
@@ -1362,7 +1378,9 @@
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="6"/>
+      <c r="B11" s="10">
+        <v>0</v>
+      </c>
       <c r="C11" s="9">
         <v>1</v>
       </c>
@@ -1407,7 +1425,9 @@
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="10">
+        <v>0</v>
+      </c>
       <c r="C12" s="9">
         <v>1</v>
       </c>
@@ -1452,7 +1472,9 @@
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="6"/>
+      <c r="B13" s="10">
+        <v>0</v>
+      </c>
       <c r="C13" s="9">
         <v>3</v>
       </c>
@@ -1497,7 +1519,9 @@
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="10">
+        <v>0</v>
+      </c>
       <c r="C14" s="9">
         <v>2</v>
       </c>
@@ -1542,7 +1566,9 @@
       <c r="A15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="6"/>
+      <c r="B15" s="10">
+        <v>0</v>
+      </c>
       <c r="C15" s="9">
         <v>1</v>
       </c>
@@ -1587,7 +1613,9 @@
       <c r="A16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="6"/>
+      <c r="B16" s="10">
+        <v>0</v>
+      </c>
       <c r="C16" s="9">
         <v>0</v>
       </c>
@@ -1632,7 +1660,9 @@
       <c r="A17" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="6"/>
+      <c r="B17" s="10">
+        <v>0</v>
+      </c>
       <c r="C17" s="9">
         <v>0</v>
       </c>
@@ -1677,7 +1707,9 @@
       <c r="A18" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="6"/>
+      <c r="B18" s="10">
+        <v>0</v>
+      </c>
       <c r="C18" s="9">
         <v>2</v>
       </c>
@@ -1722,7 +1754,9 @@
       <c r="A19" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="6"/>
+      <c r="B19" s="10">
+        <v>0</v>
+      </c>
       <c r="C19" s="9">
         <v>1</v>
       </c>
@@ -1767,7 +1801,9 @@
       <c r="A20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="6"/>
+      <c r="B20" s="10">
+        <v>0</v>
+      </c>
       <c r="C20" s="9">
         <v>0</v>
       </c>
@@ -1812,7 +1848,9 @@
       <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="10"/>
+      <c r="B21" s="10">
+        <v>0</v>
+      </c>
       <c r="C21" s="9">
         <v>0</v>
       </c>
@@ -1857,7 +1895,9 @@
       <c r="A22" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="10"/>
+      <c r="B22" s="10">
+        <v>0</v>
+      </c>
       <c r="C22" s="9">
         <v>2</v>
       </c>
@@ -1902,7 +1942,9 @@
       <c r="A23" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="10"/>
+      <c r="B23" s="10">
+        <v>0</v>
+      </c>
       <c r="C23" s="9">
         <v>4</v>
       </c>
@@ -1947,7 +1989,9 @@
       <c r="A24" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="10"/>
+      <c r="B24" s="10">
+        <v>0</v>
+      </c>
       <c r="C24" s="9">
         <v>1</v>
       </c>
@@ -1992,7 +2036,9 @@
       <c r="A25" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="10"/>
+      <c r="B25" s="10">
+        <v>0</v>
+      </c>
       <c r="C25" s="9">
         <v>3</v>
       </c>
@@ -2037,7 +2083,9 @@
       <c r="A26" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="10"/>
+      <c r="B26" s="10">
+        <v>0</v>
+      </c>
       <c r="C26" s="9">
         <v>0</v>
       </c>
@@ -2082,8 +2130,10 @@
       <c r="A27" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="15">
+      <c r="B27" s="10">
+        <v>0</v>
+      </c>
+      <c r="C27" s="12">
         <v>0</v>
       </c>
       <c r="D27">
@@ -2127,7 +2177,9 @@
       <c r="A28" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="10"/>
+      <c r="B28" s="10">
+        <v>0</v>
+      </c>
       <c r="C28" s="11">
         <v>0</v>
       </c>
@@ -2172,7 +2224,9 @@
       <c r="A29" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="10"/>
+      <c r="B29" s="10">
+        <v>0</v>
+      </c>
       <c r="C29" s="11">
         <v>1</v>
       </c>
@@ -2217,7 +2271,9 @@
       <c r="A30" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="5"/>
+      <c r="B30" s="10">
+        <v>0</v>
+      </c>
       <c r="C30" s="11">
         <v>2</v>
       </c>
@@ -2262,7 +2318,9 @@
       <c r="A31" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="5"/>
+      <c r="B31" s="10">
+        <v>0</v>
+      </c>
       <c r="C31" s="11">
         <v>1</v>
       </c>
@@ -2307,7 +2365,9 @@
       <c r="A32" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="5"/>
+      <c r="B32" s="10">
+        <v>0</v>
+      </c>
       <c r="C32" s="11">
         <v>1</v>
       </c>
@@ -2352,13 +2412,15 @@
       <c r="A33" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="5"/>
+      <c r="B33" s="10">
+        <v>1</v>
+      </c>
       <c r="C33" s="11">
         <v>3</v>
       </c>
       <c r="D33">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E33">
         <f t="shared" si="0"/>
@@ -2374,11 +2436,11 @@
       </c>
       <c r="H33">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33">
         <f t="shared" si="5"/>
@@ -2397,7 +2459,9 @@
       <c r="A34" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B34" s="5"/>
+      <c r="B34" s="10">
+        <v>0</v>
+      </c>
       <c r="C34" s="11">
         <v>1</v>
       </c>
@@ -2442,25 +2506,27 @@
       <c r="A35" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B35" s="5"/>
+      <c r="B35" s="10">
+        <v>1</v>
+      </c>
       <c r="C35" s="11">
         <v>1</v>
       </c>
       <c r="D35">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35">
-        <f t="shared" ref="E35:E66" si="11">IF(D35=0, 1,0)</f>
+        <f t="shared" ref="E35:E51" si="11">IF(D35=0, 1,0)</f>
         <v>0</v>
       </c>
       <c r="F35">
         <f t="shared" ref="F35:F51" si="12">IF(D35=1, 1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G35">
         <f t="shared" ref="G35:G51" si="13">IF(D35=2, 1, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35">
         <f t="shared" ref="H35:H51" si="14">IF(D35=3, 1, 0)</f>
@@ -2476,18 +2542,20 @@
       </c>
       <c r="K35" s="3">
         <f t="shared" ref="K35:K51" si="17">IF(D35=1,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L35" s="3">
         <f t="shared" ref="L35:L51" si="18">IF(D35&gt;1, 1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B36" s="5"/>
+      <c r="B36" s="10">
+        <v>0</v>
+      </c>
       <c r="C36" s="11">
         <v>1</v>
       </c>
@@ -2532,21 +2600,23 @@
       <c r="A37" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B37" s="5"/>
+      <c r="B37" s="10">
+        <v>1</v>
+      </c>
       <c r="C37" s="11">
         <v>0</v>
       </c>
       <c r="D37">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37">
         <f t="shared" si="13"/>
@@ -2566,7 +2636,7 @@
       </c>
       <c r="K37" s="3">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L37" s="3">
         <f t="shared" si="18"/>
@@ -2577,7 +2647,9 @@
       <c r="A38" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="5"/>
+      <c r="B38" s="10">
+        <v>0</v>
+      </c>
       <c r="C38" s="11">
         <v>0</v>
       </c>
@@ -2622,7 +2694,9 @@
       <c r="A39" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="5"/>
+      <c r="B39" s="10">
+        <v>0</v>
+      </c>
       <c r="C39" s="11">
         <v>1</v>
       </c>
@@ -2667,7 +2741,9 @@
       <c r="A40" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B40" s="5"/>
+      <c r="B40" s="10">
+        <v>0</v>
+      </c>
       <c r="C40" s="11">
         <v>1</v>
       </c>
@@ -2712,7 +2788,9 @@
       <c r="A41" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="5"/>
+      <c r="B41" s="10">
+        <v>0</v>
+      </c>
       <c r="C41" s="11">
         <v>0</v>
       </c>
@@ -2757,13 +2835,15 @@
       <c r="A42" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B42" s="5"/>
+      <c r="B42" s="5">
+        <v>1</v>
+      </c>
       <c r="C42" s="11">
         <v>4</v>
       </c>
       <c r="D42">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E42">
         <f t="shared" si="11"/>
@@ -2783,11 +2863,11 @@
       </c>
       <c r="I42">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K42" s="3">
         <f t="shared" si="17"/>
@@ -2802,7 +2882,9 @@
       <c r="A43" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B43" s="5"/>
+      <c r="B43" s="5">
+        <v>0</v>
+      </c>
       <c r="C43" s="11">
         <v>1</v>
       </c>
@@ -2847,7 +2929,9 @@
       <c r="A44" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B44" s="5"/>
+      <c r="B44" s="5">
+        <v>0</v>
+      </c>
       <c r="C44" s="11">
         <v>2</v>
       </c>
@@ -2892,7 +2976,9 @@
       <c r="A45" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B45" s="5"/>
+      <c r="B45" s="5">
+        <v>0</v>
+      </c>
       <c r="C45" s="11">
         <v>2</v>
       </c>
@@ -2937,7 +3023,9 @@
       <c r="A46" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B46" s="5"/>
+      <c r="B46" s="5">
+        <v>0</v>
+      </c>
       <c r="C46" s="11">
         <v>4</v>
       </c>
@@ -2982,7 +3070,9 @@
       <c r="A47" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B47" s="5"/>
+      <c r="B47" s="5">
+        <v>0</v>
+      </c>
       <c r="C47" s="11">
         <v>2</v>
       </c>
@@ -3027,7 +3117,9 @@
       <c r="A48" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B48" s="5"/>
+      <c r="B48" s="5">
+        <v>0</v>
+      </c>
       <c r="C48" s="11">
         <v>1</v>
       </c>
@@ -3072,7 +3164,9 @@
       <c r="A49" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B49" s="5"/>
+      <c r="B49" s="5">
+        <v>0</v>
+      </c>
       <c r="C49" s="11">
         <v>2</v>
       </c>
@@ -3117,7 +3211,9 @@
       <c r="A50" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B50" s="5"/>
+      <c r="B50" s="5">
+        <v>0</v>
+      </c>
       <c r="C50" s="11">
         <v>0</v>
       </c>
@@ -3162,7 +3258,9 @@
       <c r="A51" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B51" s="5"/>
+      <c r="B51" s="5">
+        <v>0</v>
+      </c>
       <c r="C51" s="11">
         <v>0</v>
       </c>
@@ -3207,7 +3305,9 @@
       <c r="A52" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B52" s="5"/>
+      <c r="B52" s="5">
+        <v>0</v>
+      </c>
       <c r="C52" s="11">
         <v>2</v>
       </c>
@@ -3252,7 +3352,9 @@
       <c r="A53" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B53" s="5"/>
+      <c r="B53" s="5">
+        <v>0</v>
+      </c>
       <c r="C53" s="11">
         <v>2</v>
       </c>
@@ -3297,13 +3399,15 @@
       <c r="A54" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B54" s="5"/>
+      <c r="B54" s="5">
+        <v>1</v>
+      </c>
       <c r="C54" s="11">
         <v>3</v>
       </c>
       <c r="D54">
         <f t="shared" si="19"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E54">
         <f t="shared" si="20"/>
@@ -3319,11 +3423,11 @@
       </c>
       <c r="H54">
         <f t="shared" si="23"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I54">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J54">
         <f t="shared" si="25"/>
@@ -3342,7 +3446,9 @@
       <c r="A55" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B55" s="5"/>
+      <c r="B55" s="5">
+        <v>0</v>
+      </c>
       <c r="C55" s="11">
         <v>1</v>
       </c>
@@ -3387,7 +3493,9 @@
       <c r="A56" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B56" s="5"/>
+      <c r="B56" s="5">
+        <v>0</v>
+      </c>
       <c r="C56" s="11">
         <v>5</v>
       </c>
@@ -3432,7 +3540,9 @@
       <c r="A57" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B57" s="5"/>
+      <c r="B57" s="5">
+        <v>0</v>
+      </c>
       <c r="C57" s="11">
         <v>4</v>
       </c>
@@ -3477,7 +3587,9 @@
       <c r="A58" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B58" s="5"/>
+      <c r="B58" s="5">
+        <v>0</v>
+      </c>
       <c r="C58" s="11">
         <v>2</v>
       </c>
@@ -3522,7 +3634,9 @@
       <c r="A59" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B59" s="5"/>
+      <c r="B59" s="5">
+        <v>0</v>
+      </c>
       <c r="C59" s="11">
         <v>0</v>
       </c>
@@ -3567,7 +3681,9 @@
       <c r="A60" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B60" s="5"/>
+      <c r="B60" s="5">
+        <v>0</v>
+      </c>
       <c r="C60" s="11">
         <v>2</v>
       </c>
@@ -3612,13 +3728,15 @@
       <c r="A61" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B61" s="5"/>
+      <c r="B61" s="5">
+        <v>1</v>
+      </c>
       <c r="C61" s="11">
         <v>2</v>
       </c>
       <c r="D61">
         <f t="shared" si="19"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E61">
         <f t="shared" si="20"/>
@@ -3630,11 +3748,11 @@
       </c>
       <c r="G61">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H61">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I61">
         <f t="shared" si="24"/>
@@ -3657,13 +3775,15 @@
       <c r="A62" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B62" s="5"/>
+      <c r="B62" s="5">
+        <v>1</v>
+      </c>
       <c r="C62" s="11">
         <v>2</v>
       </c>
       <c r="D62">
         <f t="shared" si="19"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E62">
         <f t="shared" si="20"/>
@@ -3675,11 +3795,11 @@
       </c>
       <c r="G62">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H62">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I62">
         <f t="shared" si="24"/>
@@ -3702,7 +3822,9 @@
       <c r="A63" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B63" s="5"/>
+      <c r="B63" s="5">
+        <v>0</v>
+      </c>
       <c r="C63" s="11">
         <v>2</v>
       </c>
@@ -3747,7 +3869,9 @@
       <c r="A64" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B64" s="5"/>
+      <c r="B64" s="5">
+        <v>0</v>
+      </c>
       <c r="C64" s="11">
         <v>1</v>
       </c>
@@ -3792,7 +3916,9 @@
       <c r="A65" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B65" s="5"/>
+      <c r="B65" s="5">
+        <v>0</v>
+      </c>
       <c r="C65" s="11">
         <v>1</v>
       </c>
@@ -3837,7 +3963,9 @@
       <c r="A66" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B66" s="5"/>
+      <c r="B66" s="5">
+        <v>0</v>
+      </c>
       <c r="C66" s="11">
         <v>0</v>
       </c>
@@ -3882,7 +4010,9 @@
       <c r="A67" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B67" s="5"/>
+      <c r="B67" s="5">
+        <v>0</v>
+      </c>
       <c r="C67" s="11">
         <v>3</v>
       </c>
@@ -3927,7 +4057,9 @@
       <c r="A68" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B68" s="5"/>
+      <c r="B68" s="5">
+        <v>0</v>
+      </c>
       <c r="C68" s="11">
         <v>1</v>
       </c>
@@ -3972,7 +4104,9 @@
       <c r="A69" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B69" s="5"/>
+      <c r="B69" s="5">
+        <v>0</v>
+      </c>
       <c r="C69" s="11">
         <v>1</v>
       </c>
@@ -4017,7 +4151,9 @@
       <c r="A70" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B70" s="5"/>
+      <c r="B70" s="5">
+        <v>0</v>
+      </c>
       <c r="C70" s="11">
         <v>2</v>
       </c>
@@ -4062,7 +4198,9 @@
       <c r="A71" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B71" s="5"/>
+      <c r="B71" s="5">
+        <v>0</v>
+      </c>
       <c r="C71" s="11">
         <v>4</v>
       </c>
@@ -4107,7 +4245,9 @@
       <c r="A72" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B72" s="5"/>
+      <c r="B72" s="5">
+        <v>0</v>
+      </c>
       <c r="C72" s="11">
         <v>2</v>
       </c>
@@ -4152,7 +4292,9 @@
       <c r="A73" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B73" s="5"/>
+      <c r="B73" s="5">
+        <v>0</v>
+      </c>
       <c r="C73" s="11">
         <v>2</v>
       </c>
@@ -4197,7 +4339,9 @@
       <c r="A74" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B74" s="5"/>
+      <c r="B74" s="5">
+        <v>0</v>
+      </c>
       <c r="C74" s="11">
         <v>2</v>
       </c>
@@ -4242,7 +4386,9 @@
       <c r="A75" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B75" s="5"/>
+      <c r="B75" s="5">
+        <v>0</v>
+      </c>
       <c r="C75" s="11">
         <v>3</v>
       </c>
@@ -4287,7 +4433,9 @@
       <c r="A76" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B76" s="5"/>
+      <c r="B76" s="5">
+        <v>0</v>
+      </c>
       <c r="C76" s="11">
         <v>2</v>
       </c>
@@ -4332,7 +4480,9 @@
       <c r="A77" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B77" s="5"/>
+      <c r="B77" s="5">
+        <v>0</v>
+      </c>
       <c r="C77" s="11">
         <v>2</v>
       </c>
@@ -4377,7 +4527,9 @@
       <c r="A78" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B78" s="5"/>
+      <c r="B78" s="5">
+        <v>0</v>
+      </c>
       <c r="C78" s="11">
         <v>4</v>
       </c>
@@ -4422,7 +4574,9 @@
       <c r="A79" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B79" s="5"/>
+      <c r="B79" s="5">
+        <v>0</v>
+      </c>
       <c r="C79" s="11">
         <v>1</v>
       </c>
@@ -4467,7 +4621,9 @@
       <c r="A80" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B80" s="5"/>
+      <c r="B80" s="5">
+        <v>0</v>
+      </c>
       <c r="C80" s="11">
         <v>1</v>
       </c>
@@ -4512,7 +4668,9 @@
       <c r="A81" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B81" s="5"/>
+      <c r="B81" s="5">
+        <v>0</v>
+      </c>
       <c r="C81" s="11">
         <v>1</v>
       </c>
@@ -4557,7 +4715,9 @@
       <c r="A82" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B82" s="5"/>
+      <c r="B82" s="5">
+        <v>0</v>
+      </c>
       <c r="C82" s="11">
         <v>1</v>
       </c>
@@ -4602,7 +4762,9 @@
       <c r="A83" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B83" s="5"/>
+      <c r="B83" s="5">
+        <v>0</v>
+      </c>
       <c r="C83" s="11">
         <v>0</v>
       </c>
@@ -4647,7 +4809,9 @@
       <c r="A84" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B84" s="5"/>
+      <c r="B84" s="5">
+        <v>0</v>
+      </c>
       <c r="C84" s="11">
         <v>1</v>
       </c>
@@ -4692,7 +4856,9 @@
       <c r="A85" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B85" s="5"/>
+      <c r="B85" s="5">
+        <v>0</v>
+      </c>
       <c r="C85" s="11">
         <v>0</v>
       </c>
@@ -4737,7 +4903,9 @@
       <c r="A86" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B86" s="8"/>
+      <c r="B86" s="5">
+        <v>0</v>
+      </c>
       <c r="C86" s="11">
         <v>2</v>
       </c>
@@ -4784,14 +4952,6 @@
     <mergeCell ref="E1:L1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B30">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="r">
-      <formula>NOT(ISERROR(SEARCH("r",B30)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="r">
-      <formula>NOT(ISERROR(SEARCH("r",B30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -4801,9 +4961,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="116" zoomScalePageLayoutView="116" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="116" zoomScaleNormal="116" zoomScalePageLayoutView="116" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3:L62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4815,21 +4975,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="E1" s="14" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="E1" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -4873,7 +5033,9 @@
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
       <c r="C3" s="3">
         <v>0</v>
       </c>
@@ -4918,7 +5080,9 @@
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
       <c r="C4" s="3">
         <v>3</v>
       </c>
@@ -4963,7 +5127,9 @@
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="5"/>
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
       <c r="C5" s="3">
         <v>0</v>
       </c>
@@ -5008,7 +5174,9 @@
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
       <c r="C6" s="4">
         <v>0</v>
       </c>
@@ -5053,7 +5221,9 @@
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
       <c r="C7" s="4">
         <v>0</v>
       </c>
@@ -5098,7 +5268,9 @@
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
       <c r="C8" s="3">
         <v>3</v>
       </c>
@@ -5143,7 +5315,9 @@
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="5">
+        <v>0</v>
+      </c>
       <c r="C9" s="4">
         <v>2</v>
       </c>
@@ -5188,7 +5362,9 @@
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="5">
+        <v>0</v>
+      </c>
       <c r="C10" s="4">
         <v>1</v>
       </c>
@@ -5233,7 +5409,9 @@
       <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
       <c r="C11" s="4">
         <v>0</v>
       </c>
@@ -5278,7 +5456,9 @@
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
       <c r="C12" s="4">
         <v>1</v>
       </c>
@@ -5323,7 +5503,9 @@
       <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="5">
+        <v>0</v>
+      </c>
       <c r="C13" s="4">
         <v>1</v>
       </c>
@@ -5368,7 +5550,9 @@
       <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="5"/>
+      <c r="B14" s="5">
+        <v>0</v>
+      </c>
       <c r="C14" s="4">
         <v>3</v>
       </c>
@@ -5413,7 +5597,9 @@
       <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="5">
+        <v>0</v>
+      </c>
       <c r="C15" s="4">
         <v>0</v>
       </c>
@@ -5458,7 +5644,9 @@
       <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="5"/>
+      <c r="B16" s="5">
+        <v>0</v>
+      </c>
       <c r="C16" s="4">
         <v>1</v>
       </c>
@@ -5503,7 +5691,9 @@
       <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="5"/>
+      <c r="B17" s="5">
+        <v>0</v>
+      </c>
       <c r="C17" s="4">
         <v>1</v>
       </c>
@@ -5548,7 +5738,9 @@
       <c r="A18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="5"/>
+      <c r="B18" s="5">
+        <v>0</v>
+      </c>
       <c r="C18" s="4">
         <v>2</v>
       </c>
@@ -5593,7 +5785,9 @@
       <c r="A19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="5"/>
+      <c r="B19" s="5">
+        <v>0</v>
+      </c>
       <c r="C19" s="4">
         <v>1</v>
       </c>
@@ -5638,7 +5832,9 @@
       <c r="A20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="5"/>
+      <c r="B20" s="5">
+        <v>0</v>
+      </c>
       <c r="C20" s="4">
         <v>2</v>
       </c>
@@ -5683,7 +5879,9 @@
       <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="5"/>
+      <c r="B21" s="5">
+        <v>0</v>
+      </c>
       <c r="C21" s="4">
         <v>1</v>
       </c>
@@ -5728,7 +5926,9 @@
       <c r="A22" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="5"/>
+      <c r="B22" s="5">
+        <v>0</v>
+      </c>
       <c r="C22" s="4">
         <v>1</v>
       </c>
@@ -5773,7 +5973,9 @@
       <c r="A23" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="5"/>
+      <c r="B23" s="5">
+        <v>0</v>
+      </c>
       <c r="C23" s="4">
         <v>2</v>
       </c>
@@ -5818,7 +6020,9 @@
       <c r="A24" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="5"/>
+      <c r="B24" s="5">
+        <v>0</v>
+      </c>
       <c r="C24" s="4">
         <v>0</v>
       </c>
@@ -5863,7 +6067,9 @@
       <c r="A25" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="5"/>
+      <c r="B25" s="5">
+        <v>0</v>
+      </c>
       <c r="C25" s="4">
         <v>1</v>
       </c>
@@ -5908,7 +6114,9 @@
       <c r="A26" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="5"/>
+      <c r="B26" s="5">
+        <v>0</v>
+      </c>
       <c r="C26" s="4">
         <v>2</v>
       </c>
@@ -5953,7 +6161,9 @@
       <c r="A27" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="5"/>
+      <c r="B27" s="5">
+        <v>0</v>
+      </c>
       <c r="C27" s="4">
         <v>2</v>
       </c>
@@ -5998,7 +6208,9 @@
       <c r="A28" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="5"/>
+      <c r="B28" s="5">
+        <v>0</v>
+      </c>
       <c r="C28" s="4">
         <v>4</v>
       </c>
@@ -6043,13 +6255,15 @@
       <c r="A29" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="5"/>
+      <c r="B29" s="5">
+        <v>1</v>
+      </c>
       <c r="C29" s="4">
         <v>3</v>
       </c>
       <c r="D29" s="3">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E29" s="3">
         <f t="shared" si="10"/>
@@ -6065,11 +6279,11 @@
       </c>
       <c r="H29">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29">
         <f t="shared" si="15"/>
@@ -6088,7 +6302,9 @@
       <c r="A30" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="5"/>
+      <c r="B30" s="5">
+        <v>0</v>
+      </c>
       <c r="C30" s="4">
         <v>2</v>
       </c>
@@ -6133,7 +6349,9 @@
       <c r="A31" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="5"/>
+      <c r="B31" s="5">
+        <v>0</v>
+      </c>
       <c r="C31" s="4">
         <v>0</v>
       </c>
@@ -6178,7 +6396,9 @@
       <c r="A32" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="5"/>
+      <c r="B32" s="5">
+        <v>0</v>
+      </c>
       <c r="C32" s="4">
         <v>0</v>
       </c>
@@ -6223,7 +6443,9 @@
       <c r="A33" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="5"/>
+      <c r="B33" s="5">
+        <v>0</v>
+      </c>
       <c r="C33" s="4">
         <v>2</v>
       </c>
@@ -6268,7 +6490,9 @@
       <c r="A34" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="5"/>
+      <c r="B34" s="5">
+        <v>0</v>
+      </c>
       <c r="C34" s="4">
         <v>0</v>
       </c>
@@ -6313,7 +6537,9 @@
       <c r="A35" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="5"/>
+      <c r="B35" s="5">
+        <v>0</v>
+      </c>
       <c r="C35" s="4">
         <v>0</v>
       </c>
@@ -6358,7 +6584,9 @@
       <c r="A36" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B36" s="2"/>
+      <c r="B36" s="5">
+        <v>0</v>
+      </c>
       <c r="C36" s="4">
         <v>2</v>
       </c>
@@ -6403,7 +6631,9 @@
       <c r="A37" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B37" s="2"/>
+      <c r="B37" s="5">
+        <v>0</v>
+      </c>
       <c r="C37" s="4">
         <v>1</v>
       </c>
@@ -6448,7 +6678,9 @@
       <c r="A38" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B38" s="2"/>
+      <c r="B38" s="5">
+        <v>0</v>
+      </c>
       <c r="C38" s="4">
         <v>0</v>
       </c>
@@ -6493,7 +6725,9 @@
       <c r="A39" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B39" s="2"/>
+      <c r="B39" s="2">
+        <v>0</v>
+      </c>
       <c r="C39" s="4" t="s">
         <v>136</v>
       </c>
@@ -6538,7 +6772,9 @@
       <c r="A40" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B40" s="2"/>
+      <c r="B40" s="2">
+        <v>0</v>
+      </c>
       <c r="C40" s="4">
         <v>1</v>
       </c>
@@ -6583,7 +6819,9 @@
       <c r="A41" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B41" s="2"/>
+      <c r="B41" s="2">
+        <v>0</v>
+      </c>
       <c r="C41" s="4">
         <v>1</v>
       </c>
@@ -6628,7 +6866,9 @@
       <c r="A42" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B42" s="2"/>
+      <c r="B42" s="2">
+        <v>0</v>
+      </c>
       <c r="C42" s="4">
         <v>0</v>
       </c>
@@ -6673,7 +6913,9 @@
       <c r="A43" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B43" s="2"/>
+      <c r="B43" s="2">
+        <v>0</v>
+      </c>
       <c r="C43" s="4">
         <v>2</v>
       </c>
@@ -6718,7 +6960,9 @@
       <c r="A44" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B44" s="2"/>
+      <c r="B44" s="2">
+        <v>0</v>
+      </c>
       <c r="C44" s="4">
         <v>3</v>
       </c>
@@ -6763,13 +7007,15 @@
       <c r="A45" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B45" s="2"/>
+      <c r="B45" s="2">
+        <v>1</v>
+      </c>
       <c r="C45" s="4">
         <v>1</v>
       </c>
       <c r="D45" s="3">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E45" s="3">
         <f t="shared" si="19"/>
@@ -6777,11 +7023,11 @@
       </c>
       <c r="F45" s="3">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G45">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45">
         <f t="shared" si="22"/>
@@ -6797,18 +7043,20 @@
       </c>
       <c r="K45">
         <f t="shared" si="25"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L45">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B46" s="2"/>
+      <c r="B46" s="2">
+        <v>0</v>
+      </c>
       <c r="C46" s="4">
         <v>4</v>
       </c>
@@ -6853,7 +7101,9 @@
       <c r="A47" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B47" s="2"/>
+      <c r="B47" s="2">
+        <v>0</v>
+      </c>
       <c r="C47" s="4">
         <v>1</v>
       </c>
@@ -6898,7 +7148,9 @@
       <c r="A48" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B48" s="2"/>
+      <c r="B48" s="2">
+        <v>0</v>
+      </c>
       <c r="C48" s="4">
         <v>1</v>
       </c>
@@ -6943,7 +7195,9 @@
       <c r="A49" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B49" s="2"/>
+      <c r="B49" s="2">
+        <v>0</v>
+      </c>
       <c r="C49" s="4">
         <v>3</v>
       </c>
@@ -6988,13 +7242,15 @@
       <c r="A50" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B50" s="2"/>
+      <c r="B50" s="2">
+        <v>2</v>
+      </c>
       <c r="C50" s="4">
         <v>1</v>
       </c>
       <c r="D50" s="3">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E50" s="3">
         <f t="shared" si="19"/>
@@ -7002,7 +7258,7 @@
       </c>
       <c r="F50" s="3">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G50">
         <f t="shared" si="21"/>
@@ -7010,7 +7266,7 @@
       </c>
       <c r="H50">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I50">
         <f t="shared" si="23"/>
@@ -7022,18 +7278,20 @@
       </c>
       <c r="K50">
         <f t="shared" si="25"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L50">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B51" s="2"/>
+      <c r="B51" s="2">
+        <v>0</v>
+      </c>
       <c r="C51" s="4">
         <v>2</v>
       </c>
@@ -7078,7 +7336,9 @@
       <c r="A52" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B52" s="2"/>
+      <c r="B52" s="2">
+        <v>0</v>
+      </c>
       <c r="C52" s="4">
         <v>2</v>
       </c>
@@ -7123,7 +7383,9 @@
       <c r="A53" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B53" s="2"/>
+      <c r="B53" s="2">
+        <v>0</v>
+      </c>
       <c r="C53" s="4">
         <v>2</v>
       </c>
@@ -7168,7 +7430,9 @@
       <c r="A54" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B54" s="2"/>
+      <c r="B54" s="2">
+        <v>0</v>
+      </c>
       <c r="C54" s="4">
         <v>1</v>
       </c>
@@ -7213,7 +7477,9 @@
       <c r="A55" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B55" s="2"/>
+      <c r="B55" s="2">
+        <v>0</v>
+      </c>
       <c r="C55" s="4">
         <v>0</v>
       </c>
@@ -7258,7 +7524,9 @@
       <c r="A56" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B56" s="2"/>
+      <c r="B56" s="2">
+        <v>0</v>
+      </c>
       <c r="C56" s="4">
         <v>1</v>
       </c>
@@ -7303,7 +7571,9 @@
       <c r="A57" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B57" s="2"/>
+      <c r="B57" s="2">
+        <v>0</v>
+      </c>
       <c r="C57" s="4">
         <v>1</v>
       </c>
@@ -7348,7 +7618,9 @@
       <c r="A58" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B58" s="2"/>
+      <c r="B58" s="2">
+        <v>0</v>
+      </c>
       <c r="C58" s="4">
         <v>1</v>
       </c>
@@ -7393,7 +7665,9 @@
       <c r="A59" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B59" s="2"/>
+      <c r="B59" s="2">
+        <v>0</v>
+      </c>
       <c r="C59" s="4">
         <v>0</v>
       </c>
@@ -7438,7 +7712,9 @@
       <c r="A60" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B60" s="2"/>
+      <c r="B60" s="2">
+        <v>0</v>
+      </c>
       <c r="C60" s="4">
         <v>0</v>
       </c>
@@ -7483,13 +7759,15 @@
       <c r="A61" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B61" s="2"/>
+      <c r="B61" s="2">
+        <v>1</v>
+      </c>
       <c r="C61" s="4">
         <v>1</v>
       </c>
       <c r="D61" s="3">
         <f t="shared" si="36"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E61" s="3">
         <f t="shared" si="37"/>
@@ -7497,11 +7775,11 @@
       </c>
       <c r="F61" s="3">
         <f t="shared" si="38"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G61">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61">
         <f t="shared" si="40"/>
@@ -7517,16 +7795,19 @@
       </c>
       <c r="K61">
         <f t="shared" si="43"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L61">
         <f t="shared" si="44"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>9.1199999999999992</v>
+      </c>
+      <c r="B62" s="2">
+        <v>0</v>
       </c>
       <c r="C62" s="4">
         <v>0</v>
@@ -7574,7 +7855,7 @@
     <mergeCell ref="E1:L1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B3:B61">
+  <conditionalFormatting sqref="B3:B62">
     <cfRule type="containsText" dxfId="0" priority="7" operator="containsText" text="r">
       <formula>NOT(ISERROR(SEARCH("r",B3)))</formula>
     </cfRule>

</xml_diff>